<commit_message>
HKD: add link to market workbook for relinkable handle
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YCSTDBootstrapping.xlsx
@@ -13,6 +13,9 @@
     <sheet name="Deposits" sheetId="6" r:id="rId4"/>
     <sheet name="Swaps" sheetId="8" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Accuracy">'General Settings'!$D$19</definedName>
     <definedName name="BondBasisDayCounter">'General Settings'!$I$15</definedName>
@@ -1292,12 +1295,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1407,6 +1404,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1435,6 +1438,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="General Settings"/>
+      <sheetName val="Hibor"/>
+      <sheetName val="Hibor Time Series"/>
+      <sheetName val="OIS"/>
+      <sheetName val="Deposits"/>
+      <sheetName val="FRA"/>
+      <sheetName val="Futures3M"/>
+      <sheetName val="Swaps1M"/>
+      <sheetName val="Swap3M"/>
+      <sheetName val="BasisSwap1M3M"/>
+      <sheetName val="BasisSwap3M6M"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="15">
+          <cell r="K15" t="str">
+            <v>HKDSTD#0000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1733,409 +1775,409 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="79" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="79" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.7109375" style="79" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="79" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.42578125" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" style="79" customWidth="1"/>
-    <col min="11" max="16384" width="8" style="79"/>
+    <col min="1" max="2" width="2.7109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="77" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="77" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="77" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.7109375" style="77" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="77" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.42578125" style="77" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="77" customWidth="1"/>
+    <col min="11" max="16384" width="8" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="79" t="str">
+      <c r="B1" s="77" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Jun 25 2014 10:33:09</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Oct 13 2014 15:51:57</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125" t="s">
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="83"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="80"/>
-      <c r="C4" s="86" t="s">
+      <c r="B4" s="78"/>
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="88" t="s">
+      <c r="E4" s="80"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="89" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="90"/>
+      <c r="I4" s="87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="80"/>
-      <c r="C5" s="91" t="s">
+      <c r="B5" s="78"/>
+      <c r="C5" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="92">
+      <c r="D5" s="90">
         <v>3</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="88" t="s">
+      <c r="E5" s="80"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="90"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="80"/>
-      <c r="C6" s="91" t="s">
+      <c r="B6" s="78"/>
+      <c r="C6" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="88" t="s">
+      <c r="E6" s="80"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="94" t="b">
+      <c r="I6" s="92" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="90"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="80"/>
-      <c r="C7" s="91" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="97"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="95"/>
     </row>
     <row r="8" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="80"/>
-      <c r="C8" s="91" t="s">
+      <c r="B8" s="78"/>
+      <c r="C8" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="82"/>
-      <c r="F8" s="124"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
-      <c r="C9" s="91" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="92" t="str">
+      <c r="D9" s="90" t="str">
         <f>Currency&amp;"_"&amp;$E$16&amp;"RH"</f>
         <v>HKD_YCSTDRH</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="125" t="s">
+      <c r="E9" s="80"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
-      <c r="J9" s="126"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="80"/>
-      <c r="C10" s="91" t="s">
+      <c r="B10" s="78"/>
+      <c r="C10" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="92" t="b">
+      <c r="D10" s="90" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="85"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="83"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="80"/>
-      <c r="C11" s="91" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="99" t="s">
+      <c r="D11" s="96"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="89" t="s">
+      <c r="I11" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="85"/>
+      <c r="J11" s="83"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="80"/>
-      <c r="C12" s="100" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="101" t="b">
+      <c r="D12" s="99" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="99" t="s">
+      <c r="E12" s="80"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="94" t="s">
+      <c r="I12" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="85"/>
+      <c r="J12" s="83"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="80"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="99" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="85"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="83"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="80"/>
-      <c r="C14" s="103" t="s">
+      <c r="B14" s="78"/>
+      <c r="C14" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="104" t="str">
+      <c r="D14" s="102" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>HKDYCSTD#0002</v>
-      </c>
-      <c r="E14" s="82"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="99" t="s">
+        <v>HKDYCSTD#0001</v>
+      </c>
+      <c r="E14" s="80"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="J14" s="85"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="83"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="80"/>
-      <c r="C15" s="105" t="s">
+      <c r="B15" s="78"/>
+      <c r="C15" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="106" t="str">
+      <c r="D15" s="104" t="str">
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
-      <c r="E15" s="107" t="s">
+      <c r="E15" s="105" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="124"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="99" t="s">
+      <c r="F15" s="122"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="85"/>
+      <c r="J15" s="83"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="80"/>
-      <c r="C16" s="103" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="108" t="str">
+      <c r="D16" s="106" t="str">
         <f>Currency&amp;$E$16</f>
         <v>HKDYCSTD</v>
       </c>
-      <c r="E16" s="109" t="s">
+      <c r="E16" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="99" t="s">
+      <c r="F16" s="122"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="89" t="s">
+      <c r="I16" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="85"/>
+      <c r="J16" s="83"/>
     </row>
     <row r="17" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="80"/>
-      <c r="C17" s="110" t="s">
+      <c r="B17" s="78"/>
+      <c r="C17" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="111">
-        <v>0</v>
-      </c>
-      <c r="E17" s="82"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="97"/>
+      <c r="D17" s="109">
+        <v>0</v>
+      </c>
+      <c r="E17" s="80"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="95"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="80"/>
-      <c r="C18" s="110" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="112" t="s">
+      <c r="D18" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="82"/>
-      <c r="F18" s="124"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="122"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="80"/>
-      <c r="C19" s="110" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="113" t="e">
+      <c r="D19" s="111" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="124"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="80"/>
-      <c r="C20" s="110" t="s">
+      <c r="B20" s="78"/>
+      <c r="C20" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="112" t="s">
+      <c r="D20" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="124"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="122"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="80"/>
-      <c r="C21" s="105" t="s">
+      <c r="B21" s="78"/>
+      <c r="C21" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="114" t="s">
+      <c r="D21" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="82"/>
-      <c r="F21" s="124"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="80"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="124"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="122"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="80"/>
-      <c r="C23" s="115">
+      <c r="B23" s="78"/>
+      <c r="C23" s="113">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41820</v>
-      </c>
-      <c r="D23" s="116">
+        <v>41943</v>
+      </c>
+      <c r="D23" s="114">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
         <v>1</v>
       </c>
-      <c r="E23" s="82"/>
-      <c r="F23" s="124"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="80"/>
-      <c r="C24" s="117">
+      <c r="B24" s="78"/>
+      <c r="C24" s="115">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>47302</v>
-      </c>
-      <c r="D24" s="92">
+        <v>49251</v>
+      </c>
+      <c r="D24" s="90">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>0.64840439763604429</v>
-      </c>
-      <c r="E24" s="82"/>
-      <c r="F24" s="124"/>
+        <v>0.57776018256954154</v>
+      </c>
+      <c r="E24" s="80"/>
+      <c r="F24" s="122"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="80"/>
-      <c r="C25" s="118" t="s">
+      <c r="B25" s="78"/>
+      <c r="C25" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="92" t="str">
+      <c r="D25" s="90" t="str">
         <f>_xll.ohRangeRetrieveError(Selected!J1)</f>
         <v/>
       </c>
-      <c r="E25" s="82"/>
-      <c r="F25" s="124"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="122"/>
     </row>
     <row r="26" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="80"/>
-      <c r="C26" s="118" t="str">
-        <f>UPPER(Currency)&amp;"STD"</f>
-        <v>HKDSTD</v>
-      </c>
-      <c r="D26" s="92" t="b">
+      <c r="B26" s="78"/>
+      <c r="C26" s="116" t="str">
+        <f>[1]Hibor!$K$15</f>
+        <v>HKDSTD#0000</v>
+      </c>
+      <c r="D26" s="90" t="b">
         <f>_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
         <v>1</v>
       </c>
-      <c r="E26" s="82"/>
-      <c r="F26" s="124"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="80"/>
-      <c r="C27" s="119" t="s">
+      <c r="B27" s="78"/>
+      <c r="C27" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="120" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="82"/>
-      <c r="F27" s="124"/>
+      <c r="D27" s="118" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="80"/>
+      <c r="F27" s="122"/>
     </row>
     <row r="28" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="121"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="122"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="124"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="122"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2218,7 +2260,7 @@
     <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>Deposits!E3</f>
-        <v>obj_00127#0002</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A2)</f>
@@ -2226,7 +2268,7 @@
       </c>
       <c r="C2" s="5">
         <f>_xll.qlRateHelperQuoteValue($A2,Trigger)</f>
-        <v>1.9857000000000004E-3</v>
+        <v>4.9790000000000001E-4</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="b">
@@ -2240,17 +2282,17 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I2" s="12">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>Deposits!E4</f>
-        <v>obj_00129#0002</v>
+        <v>obj_0013a#0001</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A3)</f>
@@ -2258,7 +2300,7 @@
       </c>
       <c r="C3" s="5">
         <f>_xll.qlRateHelperQuoteValue($A3,Trigger)</f>
-        <v>1.9285999999999999E-3</v>
+        <v>1.1357000000000001E-3</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="b">
@@ -2272,17 +2314,17 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I3" s="12">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
-        <v>41827</v>
+        <v>41950</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
         <f>Deposits!E5</f>
-        <v>obj_0012f#0002</v>
+        <v>obj_00139#0001</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A4)</f>
@@ -2290,7 +2332,7 @@
       </c>
       <c r="C4" s="5">
         <f>_xll.qlRateHelperQuoteValue($A4,Trigger)</f>
-        <v>2.0214E-3</v>
+        <v>1.5713999999999999E-3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="b">
@@ -2304,17 +2346,17 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I4" s="12">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>41834</v>
+        <v>41957</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f>Deposits!E6</f>
-        <v>obj_0012b#0002</v>
+        <v>obj_0013c#0001</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A5)</f>
@@ -2322,7 +2364,7 @@
       </c>
       <c r="C5" s="5">
         <f>_xll.qlRateHelperQuoteValue($A5,Trigger)</f>
-        <v>2.2714000000000002E-3</v>
+        <v>2.3070999999999999E-3</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="b">
@@ -2336,17 +2378,17 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I5" s="12">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
-        <v>41851</v>
+        <v>41971</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>Deposits!E7</f>
-        <v>obj_00128#0002</v>
+        <v>obj_00138#0001</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A6)</f>
@@ -2354,7 +2396,7 @@
       </c>
       <c r="C6" s="5">
         <f>_xll.qlRateHelperQuoteValue($A6,Trigger)</f>
-        <v>3.1143000000000004E-3</v>
+        <v>3.1713999999999996E-3</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="b">
@@ -2368,17 +2410,17 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($A6,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I6" s="12">
         <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
-        <v>41880</v>
+        <v>42004</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f>Deposits!E8</f>
-        <v>obj_0012c#0002</v>
+        <v>obj_0013d#0001</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A7)</f>
@@ -2386,7 +2428,7 @@
       </c>
       <c r="C7" s="5">
         <f>_xll.qlRateHelperQuoteValue($A7,Trigger)</f>
-        <v>3.7929000000000001E-3</v>
+        <v>3.7713999999999998E-3</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="b">
@@ -2400,17 +2442,17 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I7" s="12">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>41912</v>
+        <v>42034</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="str">
         <f>Deposits!E9</f>
-        <v>obj_0012a#0002</v>
+        <v>obj_0013b#0001</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A8)</f>
@@ -2418,7 +2460,7 @@
       </c>
       <c r="C8" s="5">
         <f>_xll.qlRateHelperQuoteValue($A8,Trigger)</f>
-        <v>5.5071E-3</v>
+        <v>5.3785999999999999E-3</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="b">
@@ -2432,17 +2474,17 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I8" s="12">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>42004</v>
+        <v>42124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>Deposits!E10</f>
-        <v>obj_0012d#0002</v>
+        <v>obj_0013e#0001</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A9)</f>
@@ -2464,17 +2506,17 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($A9,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I9" s="12">
         <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
-        <v>42094</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>Deposits!E11</f>
-        <v>obj_0012e#0002</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(A10)</f>
@@ -2482,7 +2524,7 @@
       </c>
       <c r="C10" s="8">
         <f>_xll.qlRateHelperQuoteValue($A10,Trigger)</f>
-        <v>8.6500000000000014E-3</v>
+        <v>8.3929E-3</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="b">
@@ -2496,17 +2538,17 @@
       </c>
       <c r="H10" s="13">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I10" s="14">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>42185</v>
+        <v>42307</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f>Swaps!K6</f>
-        <v>obj_00110#0002</v>
+        <v>obj_0011f#0001</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A11)</f>
@@ -2514,7 +2556,7 @@
       </c>
       <c r="C11" s="5">
         <f>_xll.qlRateHelperQuoteValue($A11,Trigger)</f>
-        <v>4.2000000000000006E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="D11" s="5">
         <f>_xll.qlSwapRateHelperSpread($A11,Trigger)</f>
@@ -2532,17 +2574,17 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($A11,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I11" s="12">
         <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
-        <v>42187</v>
+        <v>42311</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>Swaps!K7</f>
-        <v>obj_00122#0002</v>
+        <v>obj_00132#0001</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A12)</f>
@@ -2568,17 +2610,17 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I12" s="12">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>42279</v>
+        <v>42403</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>Swaps!K8</f>
-        <v>obj_00118#0002</v>
+        <v>obj_00125#0001</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A13)</f>
@@ -2586,7 +2628,7 @@
       </c>
       <c r="C13" s="5">
         <f>_xll.qlRateHelperQuoteValue($A13,Trigger)</f>
-        <v>5.5000000000000005E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="D13" s="5">
         <f>_xll.qlSwapRateHelperSpread($A13,Trigger)</f>
@@ -2604,17 +2646,17 @@
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I13" s="12">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
-        <v>42373</v>
+        <v>42493</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="str">
         <f>Swaps!K9</f>
-        <v>obj_0011d#0002</v>
+        <v>obj_00123#0001</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A14)</f>
@@ -2640,17 +2682,17 @@
       </c>
       <c r="H14" s="11">
         <f>_xll.qlRateHelperEarliestDate($A14,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I14" s="12">
         <f>_xll.qlRateHelperLatestDate($A14,Trigger)</f>
-        <v>42464</v>
+        <v>42585</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
         <f>Swaps!K10</f>
-        <v>obj_00114#0002</v>
+        <v>obj_00130#0001</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A15)</f>
@@ -2658,7 +2700,7 @@
       </c>
       <c r="C15" s="5">
         <f>_xll.qlRateHelperQuoteValue($A15,Trigger)</f>
-        <v>7.3000000000000001E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="D15" s="5">
         <f>_xll.qlSwapRateHelperSpread($A15,Trigger)</f>
@@ -2676,17 +2718,17 @@
       </c>
       <c r="H15" s="11">
         <f>_xll.qlRateHelperEarliestDate($A15,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I15" s="12">
         <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
-        <v>42555</v>
+        <v>42677</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
         <f>Swaps!K11</f>
-        <v>obj_00120#0002</v>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A16)</f>
@@ -2712,17 +2754,17 @@
       </c>
       <c r="H16" s="11">
         <f>_xll.qlRateHelperEarliestDate($A16,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I16" s="12">
         <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
-        <v>42920</v>
+        <v>43042</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
         <f>Swaps!K12</f>
-        <v>obj_0011e#0002</v>
+        <v>obj_00126#0001</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A17)</f>
@@ -2730,7 +2772,7 @@
       </c>
       <c r="C17" s="5">
         <f>_xll.qlRateHelperQuoteValue($A17,Trigger)</f>
-        <v>1.49E-2</v>
+        <v>1.4499999999999999E-2</v>
       </c>
       <c r="D17" s="5">
         <f>_xll.qlSwapRateHelperSpread($A17,Trigger)</f>
@@ -2748,17 +2790,17 @@
       </c>
       <c r="H17" s="11">
         <f>_xll.qlRateHelperEarliestDate($A17,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I17" s="12">
         <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
-        <v>43284</v>
+        <v>43409</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
         <f>Swaps!K13</f>
-        <v>obj_00124#0002</v>
+        <v>obj_00121#0001</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A18)</f>
@@ -2766,7 +2808,7 @@
       </c>
       <c r="C18" s="5">
         <f>_xll.qlRateHelperQuoteValue($A18,Trigger)</f>
-        <v>1.78E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="D18" s="5">
         <f>_xll.qlSwapRateHelperSpread($A18,Trigger)</f>
@@ -2784,17 +2826,17 @@
       </c>
       <c r="H18" s="11">
         <f>_xll.qlRateHelperEarliestDate($A18,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I18" s="12">
         <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
-        <v>43648</v>
+        <v>43773</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00121#0002</v>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A19)</f>
@@ -2820,17 +2862,17 @@
       </c>
       <c r="H19" s="11">
         <f>_xll.qlRateHelperEarliestDate($A19,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I19" s="12">
         <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
-        <v>44014</v>
+        <v>44138</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="str">
         <f>Swaps!K15</f>
-        <v>obj_00117#0002</v>
+        <v>obj_00122#0001</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A20)</f>
@@ -2838,7 +2880,7 @@
       </c>
       <c r="C20" s="5">
         <f>_xll.qlRateHelperQuoteValue($A20,Trigger)</f>
-        <v>2.1799999999999996E-2</v>
+        <v>2.0199999999999999E-2</v>
       </c>
       <c r="D20" s="5">
         <f>_xll.qlSwapRateHelperSpread($A20,Trigger)</f>
@@ -2856,17 +2898,17 @@
       </c>
       <c r="H20" s="11">
         <f>_xll.qlRateHelperEarliestDate($A20,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I20" s="12">
         <f>_xll.qlRateHelperLatestDate($A20,Trigger)</f>
-        <v>44379</v>
+        <v>44503</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
         <f>Swaps!K16</f>
-        <v>obj_00119#0002</v>
+        <v>obj_00129#0001</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A21)</f>
@@ -2892,17 +2934,17 @@
       </c>
       <c r="H21" s="11">
         <f>_xll.qlRateHelperEarliestDate($A21,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I21" s="12">
         <f>_xll.qlRateHelperLatestDate($A21,Trigger)</f>
-        <v>44746</v>
+        <v>44868</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
         <f>Swaps!K17</f>
-        <v>obj_00112#0002</v>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A22)</f>
@@ -2928,17 +2970,17 @@
       </c>
       <c r="H22" s="11">
         <f>_xll.qlRateHelperEarliestDate($A22,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I22" s="12">
         <f>_xll.qlRateHelperLatestDate($A22,Trigger)</f>
-        <v>45111</v>
+        <v>45233</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="str">
         <f>Swaps!K18</f>
-        <v>obj_00116#0002</v>
+        <v>obj_00120#0001</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A23)</f>
@@ -2946,7 +2988,7 @@
       </c>
       <c r="C23" s="5">
         <f>_xll.qlRateHelperQuoteValue($A23,Trigger)</f>
-        <v>2.5399999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D23" s="5">
         <f>_xll.qlSwapRateHelperSpread($A23,Trigger)</f>
@@ -2964,17 +3006,17 @@
       </c>
       <c r="H23" s="11">
         <f>_xll.qlRateHelperEarliestDate($A23,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I23" s="12">
         <f>_xll.qlRateHelperLatestDate($A23,Trigger)</f>
-        <v>45475</v>
+        <v>45600</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
         <f>Swaps!K19</f>
-        <v>obj_00125#0002</v>
+        <v>obj_00124#0001</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A24)</f>
@@ -3000,17 +3042,17 @@
       </c>
       <c r="H24" s="11">
         <f>_xll.qlRateHelperEarliestDate($A24,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I24" s="12">
         <f>_xll.qlRateHelperLatestDate($A24,Trigger)</f>
-        <v>45840</v>
+        <v>45964</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f>Swaps!K20</f>
-        <v>obj_0011c#0002</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A25)</f>
@@ -3018,7 +3060,7 @@
       </c>
       <c r="C25" s="5">
         <f>_xll.qlRateHelperQuoteValue($A25,Trigger)</f>
-        <v>2.6900000000000004E-2</v>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="D25" s="5">
         <f>_xll.qlSwapRateHelperSpread($A25,Trigger)</f>
@@ -3036,17 +3078,17 @@
       </c>
       <c r="H25" s="11">
         <f>_xll.qlRateHelperEarliestDate($A25,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I25" s="12">
         <f>_xll.qlRateHelperLatestDate($A25,Trigger)</f>
-        <v>46205</v>
+        <v>46329</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="str">
         <f>Swaps!K21</f>
-        <v>obj_00113#0002</v>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A26)</f>
@@ -3072,17 +3114,17 @@
       </c>
       <c r="H26" s="11">
         <f>_xll.qlRateHelperEarliestDate($A26,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I26" s="12">
         <f>_xll.qlRateHelperLatestDate($A26,Trigger)</f>
-        <v>46570</v>
+        <v>46694</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="str">
         <f>Swaps!K22</f>
-        <v>obj_0011a#0002</v>
+        <v>obj_0012c#0001</v>
       </c>
       <c r="B27" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A27)</f>
@@ -3108,17 +3150,17 @@
       </c>
       <c r="H27" s="11">
         <f>_xll.qlRateHelperEarliestDate($A27,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I27" s="12">
         <f>_xll.qlRateHelperLatestDate($A27,Trigger)</f>
-        <v>46938</v>
+        <v>47060</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00115#0002</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A28)</f>
@@ -3126,7 +3168,7 @@
       </c>
       <c r="C28" s="5">
         <f>_xll.qlRateHelperQuoteValue($A28,Trigger)</f>
-        <v>2.7999999999999997E-2</v>
+        <v>2.5300000000000003E-2</v>
       </c>
       <c r="D28" s="5">
         <f>_xll.qlSwapRateHelperSpread($A28,Trigger)</f>
@@ -3144,17 +3186,17 @@
       </c>
       <c r="H28" s="11">
         <f>_xll.qlRateHelperEarliestDate($A28,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I28" s="12">
         <f>_xll.qlRateHelperLatestDate($A28,Trigger)</f>
-        <v>47302</v>
+        <v>47427</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="str">
         <f>Swaps!K24</f>
-        <v>obj_00123#0002</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A29)</f>
@@ -3180,17 +3222,17 @@
       </c>
       <c r="H29" s="11">
         <f>_xll.qlRateHelperEarliestDate($A29,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I29" s="12">
         <f>_xll.qlRateHelperLatestDate($A29,Trigger)</f>
-        <v>47666</v>
+        <v>47791</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="str">
         <f>Swaps!K25</f>
-        <v>obj_0011b#0002</v>
+        <v>obj_00131#0001</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A30)</f>
@@ -3216,17 +3258,17 @@
       </c>
       <c r="H30" s="11">
         <f>_xll.qlRateHelperEarliestDate($A30,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I30" s="12">
         <f>_xll.qlRateHelperLatestDate($A30,Trigger)</f>
-        <v>48031</v>
+        <v>48155</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="str">
         <f>Swaps!K26</f>
-        <v>obj_00126#0002</v>
+        <v>obj_00127#0001</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A31)</f>
@@ -3252,17 +3294,17 @@
       </c>
       <c r="H31" s="11">
         <f>_xll.qlRateHelperEarliestDate($A31,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I31" s="12">
         <f>_xll.qlRateHelperLatestDate($A31,Trigger)</f>
-        <v>48397</v>
+        <v>48521</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="str">
         <f>Swaps!K27</f>
-        <v>obj_0011f#0002</v>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A32)</f>
@@ -3288,25 +3330,25 @@
       </c>
       <c r="H32" s="11">
         <f>_xll.qlRateHelperEarliestDate($A32,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I32" s="12">
         <f>_xll.qlRateHelperLatestDate($A32,Trigger)</f>
-        <v>48764</v>
+        <v>48886</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
         <f>Swaps!K28</f>
-        <v>obj_00111#0002</v>
+        <v>obj_00128#0001</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A33)</f>
         <v>HKDQM3H20Y_Quote</v>
       </c>
-      <c r="C33" s="5" t="e">
+      <c r="C33" s="5">
         <f>_xll.qlRateHelperQuoteValue($A33,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.6600000000000002E-2</v>
       </c>
       <c r="D33" s="5">
         <f>_xll.qlSwapRateHelperSpread($A33,Trigger)</f>
@@ -3314,7 +3356,7 @@
       </c>
       <c r="E33" s="6" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="6">
         <v>50</v>
@@ -3324,11 +3366,11 @@
       </c>
       <c r="H33" s="11">
         <f>_xll.qlRateHelperEarliestDate($A33,Trigger)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I33" s="12">
         <f>_xll.qlRateHelperLatestDate($A33,Trigger)</f>
-        <v>49129</v>
+        <v>49251</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3375,10 +3417,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="78"/>
+      <c r="B1" s="126"/>
       <c r="D1" s="15" t="s">
         <v>19</v>
       </c>
@@ -3409,7 +3451,7 @@
       </c>
       <c r="D2" s="21" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_0012a</v>
+        <v>obj_0013b</v>
       </c>
       <c r="E2" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -3417,7 +3459,7 @@
       </c>
       <c r="F2" s="22">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>5.5071E-3</v>
+        <v>5.3785999999999999E-3</v>
       </c>
       <c r="G2" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -3425,14 +3467,14 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="I2" s="28">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42004</v>
+        <v>42124</v>
       </c>
       <c r="J2" s="18">
-        <v>0.99723150393091831</v>
+        <v>0.99733989884720808</v>
       </c>
       <c r="K2" s="23"/>
     </row>
@@ -3444,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21" t="str">
-        <v>obj_00110</v>
+        <v>obj_0011f</v>
       </c>
       <c r="E3" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -3452,7 +3494,7 @@
       </c>
       <c r="F3" s="22">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.2000000000000006E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="G3" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -3460,14 +3502,14 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I3" s="28">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42187</v>
+        <v>42311</v>
       </c>
       <c r="J3" s="18">
-        <v>0.99577706452818582</v>
+        <v>0.99566169873999066</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -3479,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="str">
-        <v>obj_00118</v>
+        <v>obj_00125</v>
       </c>
       <c r="E4" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -3487,7 +3529,7 @@
       </c>
       <c r="F4" s="22">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>5.5000000000000005E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="G4" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -3495,14 +3537,14 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I4" s="28">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42373</v>
+        <v>42493</v>
       </c>
       <c r="J4" s="18">
-        <v>0.99169811311313849</v>
+        <v>0.99144452267186178</v>
       </c>
       <c r="K4" s="23"/>
     </row>
@@ -3514,7 +3556,7 @@
         <v>63</v>
       </c>
       <c r="D5" s="21" t="str">
-        <v>obj_00114</v>
+        <v>obj_00130</v>
       </c>
       <c r="E5" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -3522,7 +3564,7 @@
       </c>
       <c r="F5" s="22">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>7.3000000000000001E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="G5" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -3530,14 +3572,14 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I5" s="28">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42555</v>
+        <v>42677</v>
       </c>
       <c r="J5" s="18">
-        <v>0.98539970496567675</v>
+        <v>0.98502821458261403</v>
       </c>
       <c r="K5" s="23"/>
     </row>
@@ -3545,7 +3587,7 @@
       <c r="A6" s="54"/>
       <c r="B6" s="54"/>
       <c r="D6" s="21" t="str">
-        <v>obj_00120</v>
+        <v>obj_0012d</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -3561,20 +3603,20 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I6" s="28">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42920</v>
+        <v>43042</v>
       </c>
       <c r="J6" s="18">
-        <v>0.96641134247952087</v>
+        <v>0.96646292054688687</v>
       </c>
       <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="21" t="str">
-        <v>obj_0011e</v>
+        <v>obj_00126</v>
       </c>
       <c r="E7" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -3582,7 +3624,7 @@
       </c>
       <c r="F7" s="22">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.49E-2</v>
+        <v>1.4499999999999999E-2</v>
       </c>
       <c r="G7" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -3590,20 +3632,20 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I7" s="28">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>43284</v>
+        <v>43409</v>
       </c>
       <c r="J7" s="18">
-        <v>0.94158735841893471</v>
+        <v>0.94309882368668019</v>
       </c>
       <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="str">
-        <v>obj_00124</v>
+        <v>obj_00121</v>
       </c>
       <c r="E8" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -3611,7 +3653,7 @@
       </c>
       <c r="F8" s="22">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1.78E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G8" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -3619,20 +3661,20 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I8" s="28">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>43648</v>
+        <v>43773</v>
       </c>
       <c r="J8" s="18">
-        <v>0.91381675656223083</v>
+        <v>0.9175773083304064</v>
       </c>
       <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="21" t="str">
-        <v>obj_00117</v>
+        <v>obj_00122</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -3640,7 +3682,7 @@
       </c>
       <c r="F9" s="22">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>2.1799999999999996E-2</v>
+        <v>2.0199999999999999E-2</v>
       </c>
       <c r="G9" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -3648,20 +3690,20 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I9" s="28">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>44379</v>
+        <v>44503</v>
       </c>
       <c r="J9" s="18">
-        <v>0.8559781337806398</v>
+        <v>0.86617280980762246</v>
       </c>
       <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="21" t="str">
-        <v>obj_00116</v>
+        <v>obj_00120</v>
       </c>
       <c r="E10" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -3669,7 +3711,7 @@
       </c>
       <c r="F10" s="22">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>2.5399999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G10" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -3677,20 +3719,20 @@
       </c>
       <c r="H10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I10" s="28">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>45475</v>
+        <v>45600</v>
       </c>
       <c r="J10" s="18">
-        <v>0.7704707600219155</v>
+        <v>0.79059971098115767</v>
       </c>
       <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="21" t="str">
-        <v>obj_0011c</v>
+        <v>obj_00134</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -3698,7 +3740,7 @@
       </c>
       <c r="F11" s="22">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.6900000000000004E-2</v>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="G11" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -3706,20 +3748,20 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I11" s="28">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>46205</v>
+        <v>46329</v>
       </c>
       <c r="J11" s="18">
-        <v>0.71710513962048172</v>
+        <v>0.74277748536476151</v>
       </c>
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="str">
-        <v>obj_00115</v>
+        <v>obj_00133</v>
       </c>
       <c r="E12" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -3727,7 +3769,7 @@
       </c>
       <c r="F12" s="22">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.7999999999999997E-2</v>
+        <v>2.5300000000000003E-2</v>
       </c>
       <c r="G12" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -3735,43 +3777,43 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41822</v>
+        <v>41946</v>
       </c>
       <c r="I12" s="28">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>47302</v>
+        <v>47427</v>
       </c>
       <c r="J12" s="18">
-        <v>0.64840439763604429</v>
+        <v>0.67729530569740715</v>
       </c>
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E13" s="21" t="e">
+      <c r="D13" s="21" t="str">
+        <v>obj_00128</v>
+      </c>
+      <c r="E13" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="22" t="e">
+        <v>HKDQM3H20Y_Quote</v>
+      </c>
+      <c r="F13" s="22">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>#VALUE!</v>
+        <v>2.6600000000000002E-2</v>
       </c>
       <c r="G13" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
         <v>0</v>
       </c>
-      <c r="H13" s="11" t="e">
+      <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="28" t="e">
+        <v>41946</v>
+      </c>
+      <c r="I13" s="28">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J13" s="18" t="e">
-        <v>#N/A</v>
+        <v>49251</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0.57776018256954154</v>
       </c>
       <c r="K13" s="23"/>
     </row>
@@ -7028,7 +7070,7 @@
       </c>
       <c r="E3" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00127#0002</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="F3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -7053,7 +7095,7 @@
       </c>
       <c r="E4" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00129#0002</v>
+        <v>obj_0013a#0001</v>
       </c>
       <c r="F4" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E4)</f>
@@ -7078,7 +7120,7 @@
       </c>
       <c r="E5" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012f#0002</v>
+        <v>obj_00139#0001</v>
       </c>
       <c r="F5" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -7103,7 +7145,7 @@
       </c>
       <c r="E6" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012b#0002</v>
+        <v>obj_0013c#0001</v>
       </c>
       <c r="F6" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -7128,7 +7170,7 @@
       </c>
       <c r="E7" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00128#0002</v>
+        <v>obj_00138#0001</v>
       </c>
       <c r="F7" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -7153,7 +7195,7 @@
       </c>
       <c r="E8" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012c#0002</v>
+        <v>obj_0013d#0001</v>
       </c>
       <c r="F8" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -7178,7 +7220,7 @@
       </c>
       <c r="E9" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012a#0002</v>
+        <v>obj_0013b#0001</v>
       </c>
       <c r="F9" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -7203,7 +7245,7 @@
       </c>
       <c r="E10" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012d#0002</v>
+        <v>obj_0013e#0001</v>
       </c>
       <c r="F10" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -7228,7 +7270,7 @@
       </c>
       <c r="E11" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0012e#0002</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="F11" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -7389,7 +7431,7 @@
       <c r="J4" s="48"/>
       <c r="K4" s="63" t="str">
         <f>_xll.qlIborIndex(,FamilyName,I2,O4,Currency,P4,Q4,R4,S4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0010f#0002</v>
+        <v>obj_0011e#0001</v>
       </c>
       <c r="L4" s="64" t="str">
         <f>_xll.ohRangeRetrieveError(K4)</f>
@@ -7464,7 +7506,7 @@
       </c>
       <c r="K6" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$4,$I6,B6&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00110#0002</v>
+        <v>obj_0011f#0001</v>
       </c>
       <c r="L6" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -7507,7 +7549,7 @@
       </c>
       <c r="K7" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$4,$I7,B7&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00122#0002</v>
+        <v>obj_00132#0001</v>
       </c>
       <c r="L7" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -7550,7 +7592,7 @@
       </c>
       <c r="K8" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$4,$I8,B8&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00118#0002</v>
+        <v>obj_00125#0001</v>
       </c>
       <c r="L8" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -7593,7 +7635,7 @@
       </c>
       <c r="K9" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$4,$I9,B9&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011d#0002</v>
+        <v>obj_00123#0001</v>
       </c>
       <c r="L9" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -7636,7 +7678,7 @@
       </c>
       <c r="K10" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$4,$I10,B10&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00114#0002</v>
+        <v>obj_00130#0001</v>
       </c>
       <c r="L10" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -7679,7 +7721,7 @@
       </c>
       <c r="K11" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$4,$I11,B11&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00120#0002</v>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="L11" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -7722,7 +7764,7 @@
       </c>
       <c r="K12" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$4,$I12,B12&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011e#0002</v>
+        <v>obj_00126#0001</v>
       </c>
       <c r="L12" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -7765,7 +7807,7 @@
       </c>
       <c r="K13" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$4,$I13,B13&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00124#0002</v>
+        <v>obj_00121#0001</v>
       </c>
       <c r="L13" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -7808,7 +7850,7 @@
       </c>
       <c r="K14" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$4,$I14,B14&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00121#0002</v>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="L14" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -7851,7 +7893,7 @@
       </c>
       <c r="K15" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$4,$I15,B15&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00117#0002</v>
+        <v>obj_00122#0001</v>
       </c>
       <c r="L15" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -7894,7 +7936,7 @@
       </c>
       <c r="K16" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$4,$I16,B16&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00119#0002</v>
+        <v>obj_00129#0001</v>
       </c>
       <c r="L16" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -7937,7 +7979,7 @@
       </c>
       <c r="K17" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$4,$I17,B17&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00112#0002</v>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="L17" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -7980,7 +8022,7 @@
       </c>
       <c r="K18" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$4,$I18,B18&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00116#0002</v>
+        <v>obj_00120#0001</v>
       </c>
       <c r="L18" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -8023,7 +8065,7 @@
       </c>
       <c r="K19" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$4,$I19,B19&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00125#0002</v>
+        <v>obj_00124#0001</v>
       </c>
       <c r="L19" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -8066,7 +8108,7 @@
       </c>
       <c r="K20" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$4,$I20,B20&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011c#0002</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="L20" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -8109,7 +8151,7 @@
       </c>
       <c r="K21" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$4,$I21,B21&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00113#0002</v>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="L21" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -8152,7 +8194,7 @@
       </c>
       <c r="K22" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$4,$I22,B22&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011a#0002</v>
+        <v>obj_0012c#0001</v>
       </c>
       <c r="L22" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -8195,7 +8237,7 @@
       </c>
       <c r="K23" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$4,$I23,B23&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00115#0002</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="L23" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -8238,7 +8280,7 @@
       </c>
       <c r="K24" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$4,$I24,B24&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00123#0002</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="L24" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -8281,7 +8323,7 @@
       </c>
       <c r="K25" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$4,$I25,B25&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011b#0002</v>
+        <v>obj_00131#0001</v>
       </c>
       <c r="L25" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -8324,7 +8366,7 @@
       </c>
       <c r="K26" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$4,$I26,B26&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00126#0002</v>
+        <v>obj_00127#0001</v>
       </c>
       <c r="L26" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -8367,7 +8409,7 @@
       </c>
       <c r="K27" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$4,$I27,B27&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011f#0002</v>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="L27" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -8410,7 +8452,7 @@
       </c>
       <c r="K28" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$4,$I28,B28&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00111#0002</v>
+        <v>obj_00128#0001</v>
       </c>
       <c r="L28" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>

</xml_diff>